<commit_message>
added backdrop for header
</commit_message>
<xml_diff>
--- a/Documents/Weekly Reports/Weekly Tasks.xlsx
+++ b/Documents/Weekly Reports/Weekly Tasks.xlsx
@@ -1,139 +1,148 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="51">
   <si>
-    <t>Week</t>
-  </si>
-  <si>
-    <t>Team Member</t>
-  </si>
-  <si>
-    <t>Position(s)</t>
-  </si>
-  <si>
-    <t>Task ID</t>
-  </si>
-  <si>
-    <t>Estimated Time</t>
-  </si>
-  <si>
-    <t>Time Required</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Isaac</t>
-  </si>
-  <si>
-    <t>Technical Writing</t>
-  </si>
-  <si>
-    <t>45 Minutes</t>
-  </si>
-  <si>
-    <t>BRD - Sections 1, 2, 3 (without 3.1) and 4</t>
-  </si>
-  <si>
-    <t>2 Hours</t>
-  </si>
-  <si>
-    <t>Use case charts and editing</t>
-  </si>
-  <si>
-    <t>Database/Back-End</t>
-  </si>
-  <si>
-    <t>1 hour (total)</t>
-  </si>
-  <si>
-    <t>15 mins</t>
-  </si>
-  <si>
-    <t>database normalization/design</t>
-  </si>
-  <si>
-    <t>Jacob</t>
-  </si>
-  <si>
-    <t>30 mins</t>
-  </si>
-  <si>
-    <t>30 min</t>
-  </si>
-  <si>
-    <t>UML use cases ( C01 - C04 )</t>
-  </si>
-  <si>
-    <t>1 hour</t>
-  </si>
-  <si>
-    <t>45 min</t>
+    <t xml:space="preserve">Week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team Member</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time Required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isaac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical Writing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45 Minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRD - Sections 1, 2, 3 (without 3.1) and 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use case charts and editing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/Back-End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hour (total)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">database normalization/design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jacob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UML use cases ( C01 - C04 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45 min</t>
   </si>
   <si>
     <t xml:space="preserve">UML diagram </t>
   </si>
   <si>
-    <t>45 mins</t>
+    <t xml:space="preserve">45 mins</t>
   </si>
   <si>
     <t xml:space="preserve">BRD - UML putting all use case together </t>
   </si>
   <si>
-    <t>Brendon</t>
-  </si>
-  <si>
-    <t>Front-end</t>
-  </si>
-  <si>
-    <t>Initial website design</t>
-  </si>
-  <si>
-    <t>UI Mockup</t>
-  </si>
-  <si>
-    <t>2 hours</t>
-  </si>
-  <si>
-    <t>Gantt Chart (1st Iteration)</t>
-  </si>
-  <si>
-    <t>Ashleigh</t>
-  </si>
-  <si>
-    <t>Weekly status report, task logs</t>
-  </si>
-  <si>
-    <t>UML use case</t>
-  </si>
-  <si>
-    <t>Project Charter</t>
-  </si>
-  <si>
-    <t>Updating BRD</t>
-  </si>
-  <si>
-    <t>DataBase/Back-End</t>
+    <t xml:space="preserve">Brendon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Front-end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial website design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI Mockup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gantt Chart (1st Iteration)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashleigh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekly status report, task logs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UML use case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Charter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating BRD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataBase/Back-End</t>
   </si>
   <si>
     <t xml:space="preserve">1 hour </t>
   </si>
   <si>
-    <t>Techincal Writing</t>
-  </si>
-  <si>
-    <t>updating BRD usecases</t>
+    <t xml:space="preserve">Techincal Writing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">updating BRD usecases</t>
   </si>
   <si>
     <t xml:space="preserve">Middleware </t>
@@ -142,47 +151,79 @@
     <t xml:space="preserve">8 hours </t>
   </si>
   <si>
-    <t>3 hours</t>
-  </si>
-  <si>
-    <t>Weeb interface for entering products into database</t>
-  </si>
-  <si>
-    <t>Team Lead/Technical Writing</t>
+    <t xml:space="preserve">3 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web interface for entering products into database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team Lead/Technical Writing</t>
   </si>
   <si>
     <t xml:space="preserve">Front-end </t>
   </si>
   <si>
-    <t>4 hours</t>
-  </si>
-  <si>
-    <t>Products page</t>
-  </si>
-  <si>
-    <t>1/2 hour</t>
-  </si>
-  <si>
-    <t>Configuring Gitlab and adding progress so far</t>
+    <t xml:space="preserve">4 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Products page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2 hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuring Gitlab and adding progress so far</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="7">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -190,67 +231,106 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr fitToPage="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
+  <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="18.29"/>
-    <col customWidth="1" min="3" max="3" width="28.14"/>
-    <col customWidth="1" min="4" max="4" width="17.0"/>
-    <col customWidth="1" min="5" max="5" width="16.29"/>
-    <col customWidth="1" min="7" max="7" width="48.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="48.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -294,9 +374,9 @@
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
     </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>1.0</v>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
@@ -304,8 +384,8 @@
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3">
-        <v>6.0</v>
+      <c r="D2" s="3" t="n">
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>9</v>
@@ -317,9 +397,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="3">
-        <v>1.0</v>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
@@ -327,8 +407,8 @@
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3">
-        <v>10.0</v>
+      <c r="D3" s="3" t="n">
+        <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>11</v>
@@ -340,9 +420,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="3">
-        <v>1.0</v>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -350,8 +430,8 @@
       <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3">
-        <v>15.0</v>
+      <c r="D4" s="3" t="n">
+        <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>14</v>
@@ -363,9 +443,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="3">
-        <v>1.0</v>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
@@ -373,8 +453,8 @@
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3">
-        <v>11.0</v>
+      <c r="D5" s="3" t="n">
+        <v>11</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>18</v>
@@ -386,9 +466,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="3">
-        <v>1.0</v>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>17</v>
@@ -396,8 +476,8 @@
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3">
-        <v>7.0</v>
+      <c r="D6" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>21</v>
@@ -409,9 +489,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="3">
-        <v>1.0</v>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>17</v>
@@ -419,8 +499,8 @@
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="3">
-        <v>12.0</v>
+      <c r="D7" s="3" t="n">
+        <v>12</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>24</v>
@@ -432,9 +512,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="3">
-        <v>1.0</v>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>17</v>
@@ -442,8 +522,8 @@
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="3">
-        <v>15.0</v>
+      <c r="D8" s="3" t="n">
+        <v>15</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>14</v>
@@ -455,9 +535,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="3">
-        <v>1.0</v>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>26</v>
@@ -465,8 +545,8 @@
       <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="3">
-        <v>13.0</v>
+      <c r="D9" s="3" t="n">
+        <v>13</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>15</v>
@@ -478,9 +558,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="3">
-        <v>1.0</v>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>26</v>
@@ -488,8 +568,8 @@
       <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="3">
-        <v>14.0</v>
+      <c r="D10" s="3" t="n">
+        <v>14</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>15</v>
@@ -501,9 +581,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="3">
-        <v>1.0</v>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>26</v>
@@ -511,8 +591,8 @@
       <c r="C11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="3">
-        <v>3.0</v>
+      <c r="D11" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>21</v>
@@ -524,9 +604,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1">
-        <v>1.0</v>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>32</v>
@@ -534,8 +614,8 @@
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="1">
-        <v>17.0</v>
+      <c r="D12" s="1" t="n">
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
@@ -568,9 +648,9 @@
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
     </row>
-    <row r="13">
-      <c r="A13" s="3">
-        <v>1.0</v>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>32</v>
@@ -578,8 +658,8 @@
       <c r="C13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="3">
-        <v>15.0</v>
+      <c r="D13" s="3" t="n">
+        <v>15</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>14</v>
@@ -591,9 +671,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="3">
-        <v>1.0</v>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>32</v>
@@ -601,8 +681,8 @@
       <c r="C14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="3">
-        <v>9.0</v>
+      <c r="D14" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>18</v>
@@ -614,9 +694,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="3">
-        <v>1.0</v>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>32</v>
@@ -624,8 +704,8 @@
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="3">
-        <v>4.0</v>
+      <c r="D15" s="3" t="n">
+        <v>4</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>18</v>
@@ -637,9 +717,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="3">
-        <v>2.0</v>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>7</v>
@@ -657,9 +737,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="3">
-        <v>2.0</v>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>7</v>
@@ -677,9 +757,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="3">
-        <v>2.0</v>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>17</v>
@@ -687,8 +767,8 @@
       <c r="C18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="3">
-        <v>15.0</v>
+      <c r="D18" s="3" t="n">
+        <v>15</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>21</v>
@@ -700,9 +780,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="3">
-        <v>2.0</v>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>17</v>
@@ -710,8 +790,8 @@
       <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="3">
-        <v>11.0</v>
+      <c r="D19" s="3" t="n">
+        <v>11</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>21</v>
@@ -723,9 +803,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="3">
-        <v>2.0</v>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>17</v>
@@ -733,8 +813,8 @@
       <c r="C20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="3">
-        <v>26.0</v>
+      <c r="D20" s="3" t="n">
+        <v>26</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>42</v>
@@ -746,9 +826,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1">
-        <v>2.0</v>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>26</v>
@@ -757,9 +837,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="3">
-        <v>2.0</v>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>32</v>
@@ -778,9 +858,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="3">
-        <v>3.0</v>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>7</v>
@@ -798,16 +878,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="3"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>